<commit_message>
set default simulation to wuhan
</commit_message>
<xml_diff>
--- a/summarydataChina.xlsx
+++ b/summarydataChina.xlsx
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F10">
         <v>21</v>
@@ -600,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F11">
         <v>21</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E12">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12">
         <v>21</v>
@@ -640,10 +640,10 @@
         <v>21</v>
       </c>
       <c r="D13">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E13">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>21</v>
       </c>
       <c r="D14">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>14</v>
@@ -680,13 +680,13 @@
         <v>21</v>
       </c>
       <c r="D15">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F15">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -700,13 +700,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="E16">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="F16">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,10 +720,10 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="E17">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <v>38</v>
@@ -740,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="E18">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="F18">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -760,13 +760,13 @@
         <v>35</v>
       </c>
       <c r="D19">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="E19">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="F19">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="E20">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="F20">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,16 +797,16 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D21">
-        <v>197</v>
+        <v>231</v>
       </c>
       <c r="E21">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="F21">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -820,13 +820,13 @@
         <v>59</v>
       </c>
       <c r="D22">
-        <v>242</v>
+        <v>291</v>
       </c>
       <c r="E22">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="F22">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -834,19 +834,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C23">
+        <v>66</v>
+      </c>
+      <c r="D23">
+        <v>351</v>
+      </c>
+      <c r="E23">
+        <v>222</v>
+      </c>
+      <c r="F23">
         <v>63</v>
-      </c>
-      <c r="D23">
-        <v>283</v>
-      </c>
-      <c r="E23">
-        <v>167</v>
-      </c>
-      <c r="F23">
-        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -854,19 +854,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24">
-        <v>348</v>
+        <v>425</v>
       </c>
       <c r="E24">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="F24">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -874,19 +874,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D25">
-        <v>423</v>
+        <v>538</v>
       </c>
       <c r="E25">
-        <v>267</v>
+        <v>356</v>
       </c>
       <c r="F25">
-        <v>83</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -894,19 +894,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D26">
-        <v>514</v>
+        <v>671</v>
       </c>
       <c r="E26">
-        <v>331</v>
+        <v>454</v>
       </c>
       <c r="F26">
-        <v>97</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -914,19 +914,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D27">
-        <v>627</v>
+        <v>799</v>
       </c>
       <c r="E27">
-        <v>407</v>
+        <v>534</v>
       </c>
       <c r="F27">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -934,19 +934,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="D28">
-        <v>759</v>
+        <v>949</v>
       </c>
       <c r="E28">
-        <v>496</v>
+        <v>630</v>
       </c>
       <c r="F28">
-        <v>147</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -954,19 +954,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="D29">
-        <v>881</v>
+        <v>1142</v>
       </c>
       <c r="E29">
-        <v>574</v>
+        <v>751</v>
       </c>
       <c r="F29">
-        <v>176</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -974,19 +974,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C30">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="D30">
-        <v>1051</v>
+        <v>1352</v>
       </c>
       <c r="E30">
-        <v>667</v>
+        <v>863</v>
       </c>
       <c r="F30">
-        <v>228</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -994,19 +994,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="D31">
-        <v>1258</v>
+        <v>1610</v>
       </c>
       <c r="E31">
-        <v>781</v>
+        <v>999</v>
       </c>
       <c r="F31">
-        <v>294</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1014,19 +1014,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>220</v>
+        <v>265</v>
       </c>
       <c r="D32">
-        <v>1499</v>
+        <v>1901</v>
       </c>
       <c r="E32">
-        <v>924</v>
+        <v>1168</v>
       </c>
       <c r="F32">
-        <v>355</v>
+        <v>468</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1034,19 +1034,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <v>263</v>
+        <v>319</v>
       </c>
       <c r="D33">
-        <v>1787</v>
+        <v>2271</v>
       </c>
       <c r="E33">
-        <v>1083</v>
+        <v>1392</v>
       </c>
       <c r="F33">
-        <v>441</v>
+        <v>560</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1054,19 +1054,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>307</v>
+        <v>391</v>
       </c>
       <c r="D34">
-        <v>2148</v>
+        <v>2707</v>
       </c>
       <c r="E34">
-        <v>1330</v>
+        <v>1644</v>
       </c>
       <c r="F34">
-        <v>511</v>
+        <v>672</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1074,19 +1074,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C35">
-        <v>384</v>
+        <v>489</v>
       </c>
       <c r="D35">
-        <v>2523</v>
+        <v>3231</v>
       </c>
       <c r="E35">
-        <v>1553</v>
+        <v>1976</v>
       </c>
       <c r="F35">
-        <v>586</v>
+        <v>766</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1094,19 +1094,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C36">
-        <v>477</v>
+        <v>611</v>
       </c>
       <c r="D36">
-        <v>2980</v>
+        <v>3769</v>
       </c>
       <c r="E36">
-        <v>1828</v>
+        <v>2277</v>
       </c>
       <c r="F36">
-        <v>675</v>
+        <v>881</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1114,19 +1114,19 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C37">
-        <v>575</v>
+        <v>733</v>
       </c>
       <c r="D37">
-        <v>3469</v>
+        <v>4422</v>
       </c>
       <c r="E37">
-        <v>2075</v>
+        <v>2653</v>
       </c>
       <c r="F37">
-        <v>819</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1134,19 +1134,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C38">
-        <v>704</v>
+        <v>879</v>
       </c>
       <c r="D38">
-        <v>4076</v>
+        <v>5203</v>
       </c>
       <c r="E38">
-        <v>2433</v>
+        <v>3111</v>
       </c>
       <c r="F38">
-        <v>939</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1154,19 +1154,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C39">
-        <v>818</v>
+        <v>1063</v>
       </c>
       <c r="D39">
-        <v>4780</v>
+        <v>5968</v>
       </c>
       <c r="E39">
-        <v>2803</v>
+        <v>3474</v>
       </c>
       <c r="F39">
-        <v>1159</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1174,19 +1174,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C40">
-        <v>970</v>
+        <v>1255</v>
       </c>
       <c r="D40">
-        <v>5619</v>
+        <v>6954</v>
       </c>
       <c r="E40">
-        <v>3292</v>
+        <v>3979</v>
       </c>
       <c r="F40">
-        <v>1357</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1194,19 +1194,19 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C41">
-        <v>1152</v>
+        <v>1492</v>
       </c>
       <c r="D41">
-        <v>6617</v>
+        <v>8196</v>
       </c>
       <c r="E41">
-        <v>3859</v>
+        <v>4687</v>
       </c>
       <c r="F41">
-        <v>1606</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1214,19 +1214,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C42">
-        <v>1394</v>
+        <v>1769</v>
       </c>
       <c r="D42">
-        <v>7802</v>
+        <v>9606</v>
       </c>
       <c r="E42">
-        <v>4573</v>
+        <v>5500</v>
       </c>
       <c r="F42">
-        <v>1835</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1234,19 +1234,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C43">
-        <v>1643</v>
+        <v>2092</v>
       </c>
       <c r="D43">
-        <v>9060</v>
+        <v>11165</v>
       </c>
       <c r="E43">
-        <v>5286</v>
+        <v>6365</v>
       </c>
       <c r="F43">
-        <v>2131</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1254,19 +1254,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C44">
-        <v>1977</v>
+        <v>2494</v>
       </c>
       <c r="D44">
-        <v>10538</v>
+        <v>12887</v>
       </c>
       <c r="E44">
-        <v>6103</v>
+        <v>7269</v>
       </c>
       <c r="F44">
-        <v>2458</v>
+        <v>3124</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1274,19 +1274,19 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C45">
-        <v>2327</v>
+        <v>2975</v>
       </c>
       <c r="D45">
-        <v>12236</v>
+        <v>14876</v>
       </c>
       <c r="E45">
-        <v>7028</v>
+        <v>8376</v>
       </c>
       <c r="F45">
-        <v>2881</v>
+        <v>3525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to push back the start date to dec 3. Updated based on current infection statistics.
</commit_message>
<xml_diff>
--- a/summarydataChina.xlsx
+++ b/summarydataChina.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>21</v>
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E10">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <v>21</v>
@@ -600,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E11">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <v>21</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E12">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>21</v>
@@ -640,10 +640,10 @@
         <v>21</v>
       </c>
       <c r="D13">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E13">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -660,13 +660,13 @@
         <v>21</v>
       </c>
       <c r="D14">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="E14">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F14">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -680,13 +680,13 @@
         <v>21</v>
       </c>
       <c r="D15">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E15">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F15">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -700,13 +700,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="E16">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="F16">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="E17">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="F17">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -740,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="E18">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="F18">
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D19">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="F19">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="C20">
+        <v>36</v>
+      </c>
+      <c r="D20">
+        <v>107</v>
+      </c>
+      <c r="E20">
         <v>46</v>
       </c>
-      <c r="D20">
-        <v>195</v>
-      </c>
-      <c r="E20">
-        <v>118</v>
-      </c>
       <c r="F20">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,16 +797,16 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D21">
-        <v>231</v>
+        <v>122</v>
       </c>
       <c r="E21">
-        <v>134</v>
+        <v>51</v>
       </c>
       <c r="F21">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -817,16 +817,16 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D22">
-        <v>291</v>
+        <v>145</v>
       </c>
       <c r="E22">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="F22">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -834,19 +834,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D23">
-        <v>351</v>
+        <v>177</v>
       </c>
       <c r="E23">
-        <v>222</v>
+        <v>92</v>
       </c>
       <c r="F23">
-        <v>63</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -854,19 +854,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="D24">
-        <v>425</v>
+        <v>205</v>
       </c>
       <c r="E24">
-        <v>267</v>
+        <v>111</v>
       </c>
       <c r="F24">
-        <v>90</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -874,19 +874,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D25">
-        <v>538</v>
+        <v>233</v>
       </c>
       <c r="E25">
-        <v>356</v>
+        <v>130</v>
       </c>
       <c r="F25">
-        <v>105</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -894,19 +894,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D26">
-        <v>671</v>
+        <v>261</v>
       </c>
       <c r="E26">
-        <v>454</v>
+        <v>145</v>
       </c>
       <c r="F26">
-        <v>120</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -914,19 +914,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="D27">
-        <v>799</v>
+        <v>298</v>
       </c>
       <c r="E27">
-        <v>534</v>
+        <v>161</v>
       </c>
       <c r="F27">
-        <v>152</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -934,19 +934,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="D28">
-        <v>949</v>
+        <v>345</v>
       </c>
       <c r="E28">
-        <v>630</v>
+        <v>182</v>
       </c>
       <c r="F28">
-        <v>190</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -954,19 +954,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="D29">
-        <v>1142</v>
+        <v>410</v>
       </c>
       <c r="E29">
-        <v>751</v>
+        <v>217</v>
       </c>
       <c r="F29">
-        <v>233</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -974,19 +974,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="D30">
-        <v>1352</v>
+        <v>488</v>
       </c>
       <c r="E30">
-        <v>863</v>
+        <v>269</v>
       </c>
       <c r="F30">
-        <v>307</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -994,19 +994,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>217</v>
+        <v>116</v>
       </c>
       <c r="D31">
-        <v>1610</v>
+        <v>546</v>
       </c>
       <c r="E31">
-        <v>999</v>
+        <v>297</v>
       </c>
       <c r="F31">
-        <v>394</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1014,19 +1014,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C32">
-        <v>265</v>
+        <v>137</v>
       </c>
       <c r="D32">
-        <v>1901</v>
+        <v>627</v>
       </c>
       <c r="E32">
-        <v>1168</v>
+        <v>352</v>
       </c>
       <c r="F32">
-        <v>468</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1034,19 +1034,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>319</v>
+        <v>163</v>
       </c>
       <c r="D33">
-        <v>2271</v>
+        <v>708</v>
       </c>
       <c r="E33">
-        <v>1392</v>
+        <v>385</v>
       </c>
       <c r="F33">
-        <v>560</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1054,19 +1054,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>391</v>
+        <v>193</v>
       </c>
       <c r="D34">
-        <v>2707</v>
+        <v>799</v>
       </c>
       <c r="E34">
-        <v>1644</v>
+        <v>421</v>
       </c>
       <c r="F34">
-        <v>672</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1074,19 +1074,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>489</v>
+        <v>219</v>
       </c>
       <c r="D35">
-        <v>3231</v>
+        <v>921</v>
       </c>
       <c r="E35">
-        <v>1976</v>
+        <v>469</v>
       </c>
       <c r="F35">
-        <v>766</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1094,19 +1094,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>611</v>
+        <v>249</v>
       </c>
       <c r="D36">
-        <v>3769</v>
+        <v>1067</v>
       </c>
       <c r="E36">
-        <v>2277</v>
+        <v>542</v>
       </c>
       <c r="F36">
-        <v>881</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1114,19 +1114,19 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C37">
-        <v>733</v>
+        <v>275</v>
       </c>
       <c r="D37">
-        <v>4422</v>
+        <v>1219</v>
       </c>
       <c r="E37">
-        <v>2653</v>
+        <v>626</v>
       </c>
       <c r="F37">
-        <v>1036</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1134,19 +1134,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C38">
-        <v>879</v>
+        <v>323</v>
       </c>
       <c r="D38">
-        <v>5203</v>
+        <v>1399</v>
       </c>
       <c r="E38">
-        <v>3111</v>
+        <v>739</v>
       </c>
       <c r="F38">
-        <v>1213</v>
+        <v>337</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1154,19 +1154,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C39">
-        <v>1063</v>
+        <v>378</v>
       </c>
       <c r="D39">
-        <v>5968</v>
+        <v>1572</v>
       </c>
       <c r="E39">
-        <v>3474</v>
+        <v>820</v>
       </c>
       <c r="F39">
-        <v>1431</v>
+        <v>374</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1174,19 +1174,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C40">
-        <v>1255</v>
+        <v>452</v>
       </c>
       <c r="D40">
-        <v>6954</v>
+        <v>1785</v>
       </c>
       <c r="E40">
-        <v>3979</v>
+        <v>922</v>
       </c>
       <c r="F40">
-        <v>1720</v>
+        <v>411</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1194,19 +1194,19 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>1492</v>
+        <v>525</v>
       </c>
       <c r="D41">
-        <v>8196</v>
+        <v>2007</v>
       </c>
       <c r="E41">
-        <v>4687</v>
+        <v>998</v>
       </c>
       <c r="F41">
-        <v>2017</v>
+        <v>484</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1214,19 +1214,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>1769</v>
+        <v>593</v>
       </c>
       <c r="D42">
-        <v>9606</v>
+        <v>2294</v>
       </c>
       <c r="E42">
-        <v>5500</v>
+        <v>1139</v>
       </c>
       <c r="F42">
-        <v>2337</v>
+        <v>562</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1234,19 +1234,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C43">
-        <v>2092</v>
+        <v>660</v>
       </c>
       <c r="D43">
-        <v>11165</v>
+        <v>2583</v>
       </c>
       <c r="E43">
-        <v>6365</v>
+        <v>1270</v>
       </c>
       <c r="F43">
-        <v>2708</v>
+        <v>653</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1254,19 +1254,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C44">
-        <v>2494</v>
+        <v>752</v>
       </c>
       <c r="D44">
-        <v>12887</v>
+        <v>2931</v>
       </c>
       <c r="E44">
-        <v>7269</v>
+        <v>1455</v>
       </c>
       <c r="F44">
-        <v>3124</v>
+        <v>724</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1274,19 +1274,279 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="C45">
-        <v>2975</v>
+        <v>863</v>
       </c>
       <c r="D45">
-        <v>14876</v>
+        <v>3329</v>
       </c>
       <c r="E45">
-        <v>8376</v>
+        <v>1667</v>
       </c>
       <c r="F45">
-        <v>3525</v>
+        <v>799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>21</v>
+      </c>
+      <c r="C46">
+        <v>1009</v>
+      </c>
+      <c r="D46">
+        <v>3781</v>
+      </c>
+      <c r="E46">
+        <v>1896</v>
+      </c>
+      <c r="F46">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>23</v>
+      </c>
+      <c r="C47">
+        <v>1155</v>
+      </c>
+      <c r="D47">
+        <v>4285</v>
+      </c>
+      <c r="E47">
+        <v>2132</v>
+      </c>
+      <c r="F47">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>27</v>
+      </c>
+      <c r="C48">
+        <v>1313</v>
+      </c>
+      <c r="D48">
+        <v>4827</v>
+      </c>
+      <c r="E48">
+        <v>2381</v>
+      </c>
+      <c r="F48">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>34</v>
+      </c>
+      <c r="C49">
+        <v>1476</v>
+      </c>
+      <c r="D49">
+        <v>5441</v>
+      </c>
+      <c r="E49">
+        <v>2666</v>
+      </c>
+      <c r="F49">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>1662</v>
+      </c>
+      <c r="D50">
+        <v>6166</v>
+      </c>
+      <c r="E50">
+        <v>3041</v>
+      </c>
+      <c r="F50">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>43</v>
+      </c>
+      <c r="C51">
+        <v>1885</v>
+      </c>
+      <c r="D51">
+        <v>6941</v>
+      </c>
+      <c r="E51">
+        <v>3396</v>
+      </c>
+      <c r="F51">
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>48</v>
+      </c>
+      <c r="C52">
+        <v>2153</v>
+      </c>
+      <c r="D52">
+        <v>7801</v>
+      </c>
+      <c r="E52">
+        <v>3780</v>
+      </c>
+      <c r="F52">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>53</v>
+      </c>
+      <c r="C53">
+        <v>2446</v>
+      </c>
+      <c r="D53">
+        <v>8806</v>
+      </c>
+      <c r="E53">
+        <v>4238</v>
+      </c>
+      <c r="F53">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>62</v>
+      </c>
+      <c r="C54">
+        <v>2775</v>
+      </c>
+      <c r="D54">
+        <v>9941</v>
+      </c>
+      <c r="E54">
+        <v>4819</v>
+      </c>
+      <c r="F54">
+        <v>2347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>71</v>
+      </c>
+      <c r="C55">
+        <v>3125</v>
+      </c>
+      <c r="D55">
+        <v>11100</v>
+      </c>
+      <c r="E55">
+        <v>5306</v>
+      </c>
+      <c r="F55">
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>90</v>
+      </c>
+      <c r="C56">
+        <v>3545</v>
+      </c>
+      <c r="D56">
+        <v>12327</v>
+      </c>
+      <c r="E56">
+        <v>5764</v>
+      </c>
+      <c r="F56">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>106</v>
+      </c>
+      <c r="C57">
+        <v>4021</v>
+      </c>
+      <c r="D57">
+        <v>13691</v>
+      </c>
+      <c r="E57">
+        <v>6288</v>
+      </c>
+      <c r="F57">
+        <v>3382</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>118</v>
+      </c>
+      <c r="C58">
+        <v>4568</v>
+      </c>
+      <c r="D58">
+        <v>15165</v>
+      </c>
+      <c r="E58">
+        <v>6831</v>
+      </c>
+      <c r="F58">
+        <v>3766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated stats based on changes in china. Spreading faster mortality is lower, but this could all be an artifact of the virus infecting new populations in china.
</commit_message>
<xml_diff>
--- a/summarydataChina.xlsx
+++ b/summarydataChina.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <v>21</v>
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10">
         <v>21</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F12">
         <v>21</v>
@@ -640,10 +640,10 @@
         <v>21</v>
       </c>
       <c r="D13">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E13">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -660,13 +660,13 @@
         <v>21</v>
       </c>
       <c r="D14">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E14">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -680,10 +680,10 @@
         <v>21</v>
       </c>
       <c r="D15">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E15">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F15">
         <v>15</v>
@@ -700,10 +700,10 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E16">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F16">
         <v>21</v>
@@ -740,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F18">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E19">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F19">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -780,13 +780,13 @@
         <v>36</v>
       </c>
       <c r="D20">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="E20">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -800,13 +800,13 @@
         <v>42</v>
       </c>
       <c r="D21">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="E21">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="F21">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -820,13 +820,13 @@
         <v>47</v>
       </c>
       <c r="D22">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="E22">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F22">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -834,19 +834,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D23">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="E23">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F23">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -854,19 +854,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E24">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F24">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -874,19 +874,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D25">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="E25">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F25">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -894,19 +894,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D26">
-        <v>261</v>
+        <v>296</v>
       </c>
       <c r="E26">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F26">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -914,19 +914,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D27">
-        <v>298</v>
+        <v>356</v>
       </c>
       <c r="E27">
-        <v>161</v>
+        <v>204</v>
       </c>
       <c r="F27">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -934,19 +934,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D28">
-        <v>345</v>
+        <v>409</v>
       </c>
       <c r="E28">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="F28">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -954,19 +954,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D29">
-        <v>410</v>
+        <v>478</v>
       </c>
       <c r="E29">
-        <v>217</v>
+        <v>284</v>
       </c>
       <c r="F29">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -974,19 +974,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D30">
-        <v>488</v>
+        <v>547</v>
       </c>
       <c r="E30">
-        <v>269</v>
+        <v>332</v>
       </c>
       <c r="F30">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -994,19 +994,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="D31">
-        <v>546</v>
+        <v>627</v>
       </c>
       <c r="E31">
-        <v>297</v>
+        <v>353</v>
       </c>
       <c r="F31">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1014,19 +1014,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D32">
-        <v>627</v>
+        <v>728</v>
       </c>
       <c r="E32">
-        <v>352</v>
+        <v>399</v>
       </c>
       <c r="F32">
-        <v>138</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1034,19 +1034,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D33">
-        <v>708</v>
+        <v>844</v>
       </c>
       <c r="E33">
-        <v>385</v>
+        <v>461</v>
       </c>
       <c r="F33">
-        <v>160</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1054,19 +1054,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C34">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D34">
-        <v>799</v>
+        <v>971</v>
       </c>
       <c r="E34">
-        <v>421</v>
+        <v>527</v>
       </c>
       <c r="F34">
-        <v>185</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1074,19 +1074,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C35">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D35">
-        <v>921</v>
+        <v>1122</v>
       </c>
       <c r="E35">
-        <v>469</v>
+        <v>619</v>
       </c>
       <c r="F35">
-        <v>233</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1094,19 +1094,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="D36">
-        <v>1067</v>
+        <v>1276</v>
       </c>
       <c r="E36">
-        <v>542</v>
+        <v>686</v>
       </c>
       <c r="F36">
-        <v>276</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1117,16 +1117,16 @@
         <v>8</v>
       </c>
       <c r="C37">
-        <v>275</v>
+        <v>329</v>
       </c>
       <c r="D37">
-        <v>1219</v>
+        <v>1479</v>
       </c>
       <c r="E37">
-        <v>626</v>
+        <v>805</v>
       </c>
       <c r="F37">
-        <v>318</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1134,19 +1134,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38">
-        <v>323</v>
+        <v>383</v>
       </c>
       <c r="D38">
-        <v>1399</v>
+        <v>1695</v>
       </c>
       <c r="E38">
-        <v>739</v>
+        <v>898</v>
       </c>
       <c r="F38">
-        <v>337</v>
+        <v>414</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1154,19 +1154,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39">
-        <v>378</v>
+        <v>444</v>
       </c>
       <c r="D39">
-        <v>1572</v>
+        <v>1923</v>
       </c>
       <c r="E39">
-        <v>820</v>
+        <v>1004</v>
       </c>
       <c r="F39">
-        <v>374</v>
+        <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1174,19 +1174,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>452</v>
+        <v>503</v>
       </c>
       <c r="D40">
-        <v>1785</v>
+        <v>2167</v>
       </c>
       <c r="E40">
-        <v>922</v>
+        <v>1116</v>
       </c>
       <c r="F40">
-        <v>411</v>
+        <v>548</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1197,16 +1197,16 @@
         <v>12</v>
       </c>
       <c r="C41">
-        <v>525</v>
+        <v>590</v>
       </c>
       <c r="D41">
-        <v>2007</v>
+        <v>2472</v>
       </c>
       <c r="E41">
-        <v>998</v>
+        <v>1282</v>
       </c>
       <c r="F41">
-        <v>484</v>
+        <v>600</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1214,19 +1214,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42">
-        <v>593</v>
+        <v>674</v>
       </c>
       <c r="D42">
-        <v>2294</v>
+        <v>2806</v>
       </c>
       <c r="E42">
-        <v>1139</v>
+        <v>1431</v>
       </c>
       <c r="F42">
-        <v>562</v>
+        <v>701</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1234,19 +1234,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C43">
-        <v>660</v>
+        <v>797</v>
       </c>
       <c r="D43">
-        <v>2583</v>
+        <v>3220</v>
       </c>
       <c r="E43">
-        <v>1270</v>
+        <v>1632</v>
       </c>
       <c r="F43">
-        <v>653</v>
+        <v>791</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1254,19 +1254,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C44">
-        <v>752</v>
+        <v>919</v>
       </c>
       <c r="D44">
-        <v>2931</v>
+        <v>3704</v>
       </c>
       <c r="E44">
-        <v>1455</v>
+        <v>1886</v>
       </c>
       <c r="F44">
-        <v>724</v>
+        <v>899</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1274,19 +1274,19 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C45">
-        <v>863</v>
+        <v>1051</v>
       </c>
       <c r="D45">
-        <v>3329</v>
+        <v>4187</v>
       </c>
       <c r="E45">
-        <v>1667</v>
+        <v>2137</v>
       </c>
       <c r="F45">
-        <v>799</v>
+        <v>999</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1294,19 +1294,19 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C46">
-        <v>1009</v>
+        <v>1190</v>
       </c>
       <c r="D46">
-        <v>3781</v>
+        <v>4732</v>
       </c>
       <c r="E46">
-        <v>1896</v>
+        <v>2418</v>
       </c>
       <c r="F46">
-        <v>876</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1314,19 +1314,19 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C47">
-        <v>1155</v>
+        <v>1375</v>
       </c>
       <c r="D47">
-        <v>4285</v>
+        <v>5368</v>
       </c>
       <c r="E47">
-        <v>2132</v>
+        <v>2722</v>
       </c>
       <c r="F47">
-        <v>998</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1334,19 +1334,19 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C48">
-        <v>1313</v>
+        <v>1588</v>
       </c>
       <c r="D48">
-        <v>4827</v>
+        <v>6103</v>
       </c>
       <c r="E48">
-        <v>2381</v>
+        <v>3075</v>
       </c>
       <c r="F48">
-        <v>1133</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1354,19 +1354,19 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C49">
-        <v>1476</v>
+        <v>1818</v>
       </c>
       <c r="D49">
-        <v>5441</v>
+        <v>6926</v>
       </c>
       <c r="E49">
-        <v>2666</v>
+        <v>3475</v>
       </c>
       <c r="F49">
-        <v>1299</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1374,19 +1374,19 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C50">
-        <v>1662</v>
+        <v>2050</v>
       </c>
       <c r="D50">
-        <v>6166</v>
+        <v>7846</v>
       </c>
       <c r="E50">
-        <v>3041</v>
+        <v>3888</v>
       </c>
       <c r="F50">
-        <v>1463</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1394,19 +1394,19 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C51">
-        <v>1885</v>
+        <v>2314</v>
       </c>
       <c r="D51">
-        <v>6941</v>
+        <v>8881</v>
       </c>
       <c r="E51">
-        <v>3396</v>
+        <v>4438</v>
       </c>
       <c r="F51">
-        <v>1660</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1414,19 +1414,19 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C52">
-        <v>2153</v>
+        <v>2646</v>
       </c>
       <c r="D52">
-        <v>7801</v>
+        <v>9996</v>
       </c>
       <c r="E52">
-        <v>3780</v>
+        <v>4948</v>
       </c>
       <c r="F52">
-        <v>1868</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1434,19 +1434,19 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C53">
-        <v>2446</v>
+        <v>3028</v>
       </c>
       <c r="D53">
-        <v>8806</v>
+        <v>11269</v>
       </c>
       <c r="E53">
-        <v>4238</v>
+        <v>5507</v>
       </c>
       <c r="F53">
-        <v>2122</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1454,19 +1454,19 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C54">
-        <v>2775</v>
+        <v>3451</v>
       </c>
       <c r="D54">
-        <v>9941</v>
+        <v>12673</v>
       </c>
       <c r="E54">
-        <v>4819</v>
+        <v>6153</v>
       </c>
       <c r="F54">
-        <v>2347</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1474,19 +1474,19 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C55">
-        <v>3125</v>
+        <v>3958</v>
       </c>
       <c r="D55">
-        <v>11100</v>
+        <v>14147</v>
       </c>
       <c r="E55">
-        <v>5306</v>
+        <v>6740</v>
       </c>
       <c r="F55">
-        <v>2669</v>
+        <v>3449</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1494,19 +1494,19 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C56">
-        <v>3545</v>
+        <v>4443</v>
       </c>
       <c r="D56">
-        <v>12327</v>
+        <v>15775</v>
       </c>
       <c r="E56">
-        <v>5764</v>
+        <v>7408</v>
       </c>
       <c r="F56">
-        <v>3018</v>
+        <v>3924</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1514,19 +1514,19 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C57">
-        <v>4021</v>
+        <v>5048</v>
       </c>
       <c r="D57">
-        <v>13691</v>
+        <v>17574</v>
       </c>
       <c r="E57">
-        <v>6288</v>
+        <v>8109</v>
       </c>
       <c r="F57">
-        <v>3382</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1534,19 +1534,39 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="C58">
-        <v>4568</v>
+        <v>5762</v>
       </c>
       <c r="D58">
-        <v>15165</v>
+        <v>19335</v>
       </c>
       <c r="E58">
-        <v>6831</v>
+        <v>8689</v>
       </c>
       <c r="F58">
-        <v>3766</v>
+        <v>4884</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>164</v>
+      </c>
+      <c r="C59">
+        <v>6520</v>
+      </c>
+      <c r="D59">
+        <v>21333</v>
+      </c>
+      <c r="E59">
+        <v>9351</v>
+      </c>
+      <c r="F59">
+        <v>5462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted to current data.  Model is at its limit the naive population pool is no longer small enough to allow for consistent modeling. I may try to double the size of population, but parameter prediction is getting wilder the greater the number of days since the beginning of the outbreak due to random drift. Hubei accounts for most of mortality some of this likely due to that city being overwhelmed and unable to care the number of people who are sick. If mortality looks drastically different in the next few days I will attempt to try to update the model.
</commit_message>
<xml_diff>
--- a/summarydataChina.xlsx
+++ b/summarydataChina.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -560,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>21</v>
@@ -580,10 +580,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E10">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>21</v>
@@ -600,10 +600,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F11">
         <v>21</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E12">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F12">
         <v>21</v>
@@ -640,10 +640,10 @@
         <v>21</v>
       </c>
       <c r="D13">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E13">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -660,13 +660,13 @@
         <v>21</v>
       </c>
       <c r="D14">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E14">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F14">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -680,13 +680,13 @@
         <v>21</v>
       </c>
       <c r="D15">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E15">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -700,13 +700,13 @@
         <v>21</v>
       </c>
       <c r="D16">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E16">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F16">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -720,13 +720,13 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E17">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F17">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -740,13 +740,13 @@
         <v>21</v>
       </c>
       <c r="D18">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E18">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F18">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,16 +757,16 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D19">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E19">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F19">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E20">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F20">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,16 +797,16 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E21">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F21">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -817,16 +817,16 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E22">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F22">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -834,19 +834,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D23">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="E23">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F23">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -854,19 +854,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D24">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="E24">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F24">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -874,19 +874,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D25">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="E25">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F25">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -894,19 +894,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E26">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F26">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -914,19 +914,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D27">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E27">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F27">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -934,19 +934,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D28">
-        <v>409</v>
+        <v>417</v>
       </c>
       <c r="E28">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="F28">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -954,19 +954,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D29">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="E29">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F29">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -974,19 +974,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C30">
         <v>116</v>
       </c>
       <c r="D30">
-        <v>547</v>
+        <v>576</v>
       </c>
       <c r="E30">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="F30">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -994,19 +994,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D31">
-        <v>627</v>
+        <v>669</v>
       </c>
       <c r="E31">
-        <v>353</v>
+        <v>397</v>
       </c>
       <c r="F31">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1014,19 +1014,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C32">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D32">
-        <v>728</v>
+        <v>751</v>
       </c>
       <c r="E32">
-        <v>399</v>
+        <v>421</v>
       </c>
       <c r="F32">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1034,19 +1034,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D33">
-        <v>844</v>
+        <v>872</v>
       </c>
       <c r="E33">
-        <v>461</v>
+        <v>478</v>
       </c>
       <c r="F33">
-        <v>206</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1054,19 +1054,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D34">
-        <v>971</v>
+        <v>1036</v>
       </c>
       <c r="E34">
-        <v>527</v>
+        <v>592</v>
       </c>
       <c r="F34">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1074,19 +1074,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="D35">
-        <v>1122</v>
+        <v>1195</v>
       </c>
       <c r="E35">
-        <v>619</v>
+        <v>665</v>
       </c>
       <c r="F35">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1094,19 +1094,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D36">
-        <v>1276</v>
+        <v>1381</v>
       </c>
       <c r="E36">
-        <v>686</v>
+        <v>754</v>
       </c>
       <c r="F36">
-        <v>316</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1114,19 +1114,19 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D37">
-        <v>1479</v>
+        <v>1610</v>
       </c>
       <c r="E37">
-        <v>805</v>
+        <v>900</v>
       </c>
       <c r="F37">
-        <v>345</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1134,19 +1134,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="D38">
-        <v>1695</v>
+        <v>1799</v>
       </c>
       <c r="E38">
-        <v>898</v>
+        <v>976</v>
       </c>
       <c r="F38">
-        <v>414</v>
+        <v>429</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1154,19 +1154,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>444</v>
       </c>
       <c r="D39">
-        <v>1923</v>
+        <v>2054</v>
       </c>
       <c r="E39">
-        <v>1004</v>
+        <v>1096</v>
       </c>
       <c r="F39">
-        <v>475</v>
+        <v>514</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1174,19 +1174,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40">
-        <v>503</v>
+        <v>530</v>
       </c>
       <c r="D40">
-        <v>2167</v>
+        <v>2356</v>
       </c>
       <c r="E40">
-        <v>1116</v>
+        <v>1241</v>
       </c>
       <c r="F40">
-        <v>548</v>
+        <v>585</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1194,19 +1194,19 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C41">
-        <v>590</v>
+        <v>627</v>
       </c>
       <c r="D41">
-        <v>2472</v>
+        <v>2749</v>
       </c>
       <c r="E41">
-        <v>1282</v>
+        <v>1450</v>
       </c>
       <c r="F41">
-        <v>600</v>
+        <v>672</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1214,19 +1214,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42">
-        <v>674</v>
+        <v>710</v>
       </c>
       <c r="D42">
-        <v>2806</v>
+        <v>3161</v>
       </c>
       <c r="E42">
-        <v>1431</v>
+        <v>1660</v>
       </c>
       <c r="F42">
-        <v>701</v>
+        <v>791</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1234,19 +1234,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C43">
-        <v>797</v>
+        <v>823</v>
       </c>
       <c r="D43">
-        <v>3220</v>
+        <v>3646</v>
       </c>
       <c r="E43">
-        <v>1632</v>
+        <v>1948</v>
       </c>
       <c r="F43">
-        <v>791</v>
+        <v>875</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1254,19 +1254,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44">
-        <v>919</v>
+        <v>958</v>
       </c>
       <c r="D44">
-        <v>3704</v>
+        <v>4159</v>
       </c>
       <c r="E44">
-        <v>1886</v>
+        <v>2219</v>
       </c>
       <c r="F44">
-        <v>899</v>
+        <v>982</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1274,19 +1274,19 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C45">
-        <v>1051</v>
+        <v>1115</v>
       </c>
       <c r="D45">
-        <v>4187</v>
+        <v>4729</v>
       </c>
       <c r="E45">
-        <v>2137</v>
+        <v>2516</v>
       </c>
       <c r="F45">
-        <v>999</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1294,19 +1294,19 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C46">
-        <v>1190</v>
+        <v>1299</v>
       </c>
       <c r="D46">
-        <v>4732</v>
+        <v>5391</v>
       </c>
       <c r="E46">
-        <v>2418</v>
+        <v>2816</v>
       </c>
       <c r="F46">
-        <v>1124</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1317,16 +1317,16 @@
         <v>27</v>
       </c>
       <c r="C47">
-        <v>1375</v>
+        <v>1501</v>
       </c>
       <c r="D47">
-        <v>5368</v>
+        <v>6153</v>
       </c>
       <c r="E47">
-        <v>2722</v>
+        <v>3175</v>
       </c>
       <c r="F47">
-        <v>1271</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1334,19 +1334,19 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C48">
-        <v>1588</v>
+        <v>1698</v>
       </c>
       <c r="D48">
-        <v>6103</v>
+        <v>7054</v>
       </c>
       <c r="E48">
-        <v>3075</v>
+        <v>3651</v>
       </c>
       <c r="F48">
-        <v>1440</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1357,16 +1357,16 @@
         <v>38</v>
       </c>
       <c r="C49">
-        <v>1818</v>
+        <v>1940</v>
       </c>
       <c r="D49">
-        <v>6926</v>
+        <v>8037</v>
       </c>
       <c r="E49">
-        <v>3475</v>
+        <v>4127</v>
       </c>
       <c r="F49">
-        <v>1633</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1374,19 +1374,19 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C50">
-        <v>2050</v>
+        <v>2213</v>
       </c>
       <c r="D50">
-        <v>7846</v>
+        <v>9170</v>
       </c>
       <c r="E50">
-        <v>3888</v>
+        <v>4739</v>
       </c>
       <c r="F50">
-        <v>1908</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1394,19 +1394,19 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51">
-        <v>2314</v>
+        <v>2575</v>
       </c>
       <c r="D51">
-        <v>8881</v>
+        <v>10397</v>
       </c>
       <c r="E51">
-        <v>4438</v>
+        <v>5319</v>
       </c>
       <c r="F51">
-        <v>2129</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1414,19 +1414,19 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C52">
-        <v>2646</v>
+        <v>2978</v>
       </c>
       <c r="D52">
-        <v>9996</v>
+        <v>11751</v>
       </c>
       <c r="E52">
-        <v>4948</v>
+        <v>5937</v>
       </c>
       <c r="F52">
-        <v>2402</v>
+        <v>2836</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1434,19 +1434,19 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C53">
-        <v>3028</v>
+        <v>3403</v>
       </c>
       <c r="D53">
-        <v>11269</v>
+        <v>13228</v>
       </c>
       <c r="E53">
-        <v>5507</v>
+        <v>6623</v>
       </c>
       <c r="F53">
-        <v>2734</v>
+        <v>3202</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1454,19 +1454,19 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C54">
-        <v>3451</v>
+        <v>3910</v>
       </c>
       <c r="D54">
-        <v>12673</v>
+        <v>14773</v>
       </c>
       <c r="E54">
-        <v>6153</v>
+        <v>7214</v>
       </c>
       <c r="F54">
-        <v>3069</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1474,19 +1474,19 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C55">
-        <v>3958</v>
+        <v>4431</v>
       </c>
       <c r="D55">
-        <v>14147</v>
+        <v>16530</v>
       </c>
       <c r="E55">
-        <v>6740</v>
+        <v>7902</v>
       </c>
       <c r="F55">
-        <v>3449</v>
+        <v>4197</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1494,79 +1494,19 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C56">
-        <v>4443</v>
+        <v>5078</v>
       </c>
       <c r="D56">
-        <v>15775</v>
+        <v>18420</v>
       </c>
       <c r="E56">
-        <v>7408</v>
+        <v>8625</v>
       </c>
       <c r="F56">
-        <v>3924</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57">
-        <v>120</v>
-      </c>
-      <c r="C57">
-        <v>5048</v>
-      </c>
-      <c r="D57">
-        <v>17574</v>
-      </c>
-      <c r="E57">
-        <v>8109</v>
-      </c>
-      <c r="F57">
-        <v>4417</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="1">
-        <v>56</v>
-      </c>
-      <c r="B58">
-        <v>143</v>
-      </c>
-      <c r="C58">
-        <v>5762</v>
-      </c>
-      <c r="D58">
-        <v>19335</v>
-      </c>
-      <c r="E58">
-        <v>8689</v>
-      </c>
-      <c r="F58">
-        <v>4884</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59">
-        <v>164</v>
-      </c>
-      <c r="C59">
-        <v>6520</v>
-      </c>
-      <c r="D59">
-        <v>21333</v>
-      </c>
-      <c r="E59">
-        <v>9351</v>
-      </c>
-      <c r="F59">
-        <v>5462</v>
+        <v>4717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>